<commit_message>
Reparos no main e atualizar sempre
</commit_message>
<xml_diff>
--- a/Files/INFORMATIVO 16° GRE - MODELO.xlsx
+++ b/Files/INFORMATIVO 16° GRE - MODELO.xlsx
@@ -90,9 +90,6 @@
     <t>NNL-7286</t>
   </si>
   <si>
-    <t>KIQ-8720</t>
-  </si>
-  <si>
     <t>SÃO JULIÃO</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>NHU-2780</t>
+  </si>
+  <si>
+    <t>KZQ-8720</t>
   </si>
 </sst>
 </file>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,8 +1111,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>23</v>
+      <c r="A30" t="s">
+        <v>38</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>6</v>
@@ -1127,12 +1127,12 @@
         <v>9</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>23</v>
+      <c r="A31" t="s">
+        <v>38</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>6</v>
@@ -1147,92 +1147,92 @@
         <v>8</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>6</v>
@@ -1247,12 +1247,12 @@
         <v>9</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>6</v>
@@ -1267,12 +1267,12 @@
         <v>8</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>6</v>
@@ -1287,12 +1287,12 @@
         <v>9</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>6</v>
@@ -1307,12 +1307,12 @@
         <v>8</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>6</v>
@@ -1327,12 +1327,12 @@
         <v>8</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>6</v>
@@ -1347,12 +1347,12 @@
         <v>9</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>6</v>
@@ -1367,12 +1367,12 @@
         <v>9</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>6</v>
@@ -1387,12 +1387,12 @@
         <v>8</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>6</v>
@@ -1407,12 +1407,12 @@
         <v>9</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>6</v>
@@ -1427,12 +1427,12 @@
         <v>8</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>6</v>
@@ -1447,12 +1447,12 @@
         <v>9</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>6</v>
@@ -1467,12 +1467,12 @@
         <v>8</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>6</v>
@@ -1487,12 +1487,12 @@
         <v>8</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>6</v>
@@ -1507,12 +1507,12 @@
         <v>9</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>6</v>
@@ -1527,12 +1527,12 @@
         <v>9</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>6</v>
@@ -1547,132 +1547,132 @@
         <v>8</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>6</v>
@@ -1687,12 +1687,12 @@
         <v>9</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>6</v>
@@ -1707,12 +1707,12 @@
         <v>8</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>6</v>
@@ -1727,12 +1727,12 @@
         <v>9</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>6</v>
@@ -1747,12 +1747,12 @@
         <v>8</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>6</v>
@@ -1767,12 +1767,12 @@
         <v>8</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>6</v>
@@ -1787,12 +1787,12 @@
         <v>9</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>6</v>
@@ -1807,12 +1807,12 @@
         <v>9</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>6</v>
@@ -1827,12 +1827,12 @@
         <v>8</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>6</v>
@@ -1847,12 +1847,12 @@
         <v>9</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>6</v>
@@ -1867,12 +1867,12 @@
         <v>8</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>6</v>
@@ -1887,12 +1887,12 @@
         <v>9</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>6</v>
@@ -1907,12 +1907,12 @@
         <v>8</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>6</v>
@@ -1927,12 +1927,12 @@
         <v>9</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>6</v>
@@ -1947,7 +1947,7 @@
         <v>8</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>